<commit_message>
implementation of "download CSV Report" on /results
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/backend/test_sales_pipelines_generated.xlsx
+++ b/backend/test_sales_pipelines_generated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewabbott/Library/CloudStorage/GoogleDrive-aabbott@gmail.com/My Drive/Andrew/RevOps/v2/revtrust/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FC7410CB-2DA0-8548-990C-1795621BB50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B51D3E2E-9053-9842-AAF8-08B1EA36BBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="900" windowWidth="28040" windowHeight="17180" xr2:uid="{DEAB22B0-42A6-1D4F-ACEA-4606DCB7BAF7}"/>
   </bookViews>
@@ -1239,10 +1239,13 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>